<commit_message>
cap nhat bang phan cong cong viec
</commit_message>
<xml_diff>
--- a/TH1/BangPhanCongCongViec.xlsx
+++ b/TH1/BangPhanCongCongViec.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAI LIEU LAP TRINH\TDMU\Nam 4\Lap trinh CSDL\DO AN CUOI KI\LTCSDL_QuanLySieuThiMini\TH1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TAI LIEU DAI HOC\HOC KI 7\LAP TRINH CO SO DU LIEU\cuoi ki\LTCSDL_QuanLySieuThiMini\TH1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A605712C-DAB3-4383-9EE6-9BBBDCE727B8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="24000" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="24000" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>STT</t>
   </si>
@@ -100,17 +99,41 @@
   </si>
   <si>
     <t>Duy, Khởi, Thiện</t>
+  </si>
+  <si>
+    <t>Thiết kế form quản lý loại hàng</t>
+  </si>
+  <si>
+    <t>THỰC HÀNH 3</t>
+  </si>
+  <si>
+    <t>Thiết kế form quản lý hàng hóa</t>
+  </si>
+  <si>
+    <t>Thiết kế form nhập hàng hóa</t>
+  </si>
+  <si>
+    <t>Khởi</t>
+  </si>
+  <si>
+    <t>Thiện</t>
+  </si>
+  <si>
+    <t>10h - 02/11/2018</t>
+  </si>
+  <si>
+    <t>10h - 26/10/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -119,13 +142,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -168,11 +197,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -197,6 +263,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -478,20 +557,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="40.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" customWidth="1"/>
-    <col min="5" max="5" width="23.59765625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
@@ -589,7 +668,7 @@
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>4</v>
       </c>
@@ -605,12 +684,14 @@
       <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -626,13 +707,75 @@
       <c r="E10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>8</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>